<commit_message>
Added GME part names for THT BOM.
</commit_message>
<xml_diff>
--- a/Fabrication output/testbench-BOM-THT-mouser.xlsx
+++ b/Fabrication output/testbench-BOM-THT-mouser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\skola\DP\DP\Fabrication output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F2853F-163D-44E0-B8DC-08F68CD5F614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93468A94-7476-4D05-8F45-44E1B65F560A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46320" yWindow="0" windowWidth="11280" windowHeight="15600" xr2:uid="{25989565-899A-4067-90CE-1940FB6E11F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25989565-899A-4067-90CE-1940FB6E11F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>Designator</t>
   </si>
@@ -147,13 +147,58 @@
   </si>
   <si>
     <t xml:space="preserve">https://cz.mouser.com/ProductDetail/Amphenol-FCI/10129378-910001BLF?qs=0lQeLiL1qyaKTim8PTf2WA%3D%3D </t>
+  </si>
+  <si>
+    <t>GME</t>
+  </si>
+  <si>
+    <t>KLS MLW10G konektor</t>
+  </si>
+  <si>
+    <t>distancni slopek plastovy 10mm</t>
+  </si>
+  <si>
+    <t>dutinkova lista 8 pin</t>
+  </si>
+  <si>
+    <t>BL104G-V5,7 dutinková lišta 1x4pin</t>
+  </si>
+  <si>
+    <t>CONNFLY S2G06C, kolikova lista 2x3 pin</t>
+  </si>
+  <si>
+    <t>CONNFLY S1G04C kolíková lišta 1x4 pin</t>
+  </si>
+  <si>
+    <t>CONNFLY S1G06C kolíková lišta 1x6</t>
+  </si>
+  <si>
+    <t>KLS BL105G-V8.5 dutinková lišta 1x5 pin</t>
+  </si>
+  <si>
+    <t>dutinková lišta 1x6pin 2.54mm roztec</t>
+  </si>
+  <si>
+    <t>CONNFLY S1G02C kolíková lišta 1x2 pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KLS S1G08C kolíková lišta 1x8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KLS S1G10C kolíková lišta 1x10</t>
+  </si>
+  <si>
+    <t>pruzinovy pogo kontakt samice</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/mill-max-manufacturing-corp/4141-0-00-15-00-00-03-0/16341759</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,13 +210,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -194,7 +232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,12 +242,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,14 +257,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -548,241 +579,290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77421293-2C68-4A39-BA08-389452BB8866}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="100.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="118.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
         <v>32</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19" s="3"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C22" s="3"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{A0D22948-E3EE-4595-A350-ECB99809285F}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{71C8353C-F9A2-4262-93B3-F5AF8945B21D}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{0B840C41-BF1B-4940-8F3F-7DCD83270BA6}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{AD873A6B-C461-4969-B854-4926A3C55A93}"/>
-    <hyperlink ref="D9" r:id="rId5" xr:uid="{31E4171E-1D6A-4C43-83AA-E643AECEDA60}"/>
-    <hyperlink ref="D5" r:id="rId6" xr:uid="{E93E18A0-924F-4827-9CE3-6D863A23D833}"/>
-    <hyperlink ref="D10" r:id="rId7" xr:uid="{93D9BCD6-E800-4F54-BD26-57F2EAE9137E}"/>
-    <hyperlink ref="D8" r:id="rId8" xr:uid="{6E22B03A-9537-4FB7-B524-95B9AE5C28E7}"/>
-    <hyperlink ref="D11" r:id="rId9" xr:uid="{9BBDD3BA-D32B-404A-B9B4-1AECD593BDFF}"/>
-    <hyperlink ref="D12" r:id="rId10" xr:uid="{99BFB79C-A893-4A87-A6B8-CD7B8A4112DB}"/>
-    <hyperlink ref="D13" r:id="rId11" xr:uid="{9CAC6F31-E5C4-488E-BD32-10DDB964BDE5}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{A0D22948-E3EE-4595-A350-ECB99809285F}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{71C8353C-F9A2-4262-93B3-F5AF8945B21D}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{0B840C41-BF1B-4940-8F3F-7DCD83270BA6}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{AD873A6B-C461-4969-B854-4926A3C55A93}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{31E4171E-1D6A-4C43-83AA-E643AECEDA60}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{E93E18A0-924F-4827-9CE3-6D863A23D833}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{93D9BCD6-E800-4F54-BD26-57F2EAE9137E}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{6E22B03A-9537-4FB7-B524-95B9AE5C28E7}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{9BBDD3BA-D32B-404A-B9B4-1AECD593BDFF}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{99BFB79C-A893-4A87-A6B8-CD7B8A4112DB}"/>
+    <hyperlink ref="E13" r:id="rId11" xr:uid="{9CAC6F31-E5C4-488E-BD32-10DDB964BDE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Edited BOM of THT parts.
</commit_message>
<xml_diff>
--- a/Fabrication output/testbench-BOM-THT-mouser.xlsx
+++ b/Fabrication output/testbench-BOM-THT-mouser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\skola\DP\DP\Fabrication output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93468A94-7476-4D05-8F45-44E1B65F560A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A754A0A-611F-4716-84D4-8D6389B74BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25989565-899A-4067-90CE-1940FB6E11F4}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{25989565-899A-4067-90CE-1940FB6E11F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>Designator</t>
   </si>
@@ -192,6 +192,24 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/mill-max-manufacturing-corp/4141-0-00-15-00-00-03-0/16341759</t>
+  </si>
+  <si>
+    <t>5 zilovy kabel</t>
+  </si>
+  <si>
+    <t>1x kabel 5 zilovy samec/samice</t>
+  </si>
+  <si>
+    <t>1x kabel 4 zilovy samice/samice</t>
+  </si>
+  <si>
+    <t>pogo piny</t>
+  </si>
+  <si>
+    <t>tme</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/cz/details/pogo-pin2mmx11.3mm/konektory-ostatni/</t>
   </si>
 </sst>
 </file>
@@ -582,7 +600,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +632,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -631,7 +649,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
@@ -651,7 +669,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
@@ -685,7 +703,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>47</v>
@@ -753,7 +771,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
         <v>43</v>
@@ -770,7 +788,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
@@ -787,7 +805,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
         <v>48</v>
@@ -804,7 +822,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
         <v>49</v>
@@ -821,7 +839,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
         <v>39</v>
@@ -829,24 +847,45 @@
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D19" s="2"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
       <c r="D22" s="2"/>
     </row>
   </sheetData>

</xml_diff>